<commit_message>
Clean version if not run on anaconda - weight enables as test feature
</commit_message>
<xml_diff>
--- a/Devices.xlsx
+++ b/Devices.xlsx
@@ -510,7 +510,7 @@
         <v>20</v>
       </c>
       <c r="G2">
-        <v>1653109149</v>
+        <v>1653195549</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>
@@ -542,7 +542,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>1653109143</v>
+        <v>1653195544</v>
       </c>
       <c r="H3" t="s">
         <v>23</v>
@@ -606,7 +606,7 @@
         <v>20</v>
       </c>
       <c r="G5">
-        <v>1653109155</v>
+        <v>1653195556</v>
       </c>
       <c r="H5" t="s">
         <v>25</v>
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
       <c r="G6">
-        <v>1653089376</v>
+        <v>1653176010</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
@@ -670,7 +670,7 @@
         <v>21</v>
       </c>
       <c r="G7">
-        <v>1653099360</v>
+        <v>1653186311</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>

</xml_diff>